<commit_message>
player table added to database
got player database working properly
</commit_message>
<xml_diff>
--- a/2024 OIA All.xlsx
+++ b/2024 OIA All.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Side Hustles\OIA Golf Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Side Hustles\OIAGolf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CB4B3D9-0F85-44D6-AFCC-3CFC9844E1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6191B89E-2E2B-46A0-82D6-DBFB2FB3294C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="730" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Scores Boys" sheetId="2" r:id="rId1"/>
@@ -1404,10 +1404,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1729,9 +1725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC9CF80-3480-4C15-90C0-DFEB0D656A8C}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5179,8 +5175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D101CC1F-9528-4CB5-AF0C-982E0736A7E9}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25205,7 +25201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F083A5E2-02EA-45F9-B8A5-EB84C60E71D2}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>